<commit_message>
The draft of the report.
</commit_message>
<xml_diff>
--- a/3.a.SentenceBert/splitSentenceBertCluster/finalGroup_8.xlsx
+++ b/3.a.SentenceBert/splitSentenceBertCluster/finalGroup_8.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,11 @@
           <t>preProcessedResult</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -457,6 +462,11 @@
           <t>群组 设置 当群 主将 请求 加入 群 策略 设置 拒绝请求 管理员 审批 成员 随意 邀请 加入 群主 管理员 并未 收到 加入 请求 信息</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>安全</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -467,6 +477,11 @@
       <c r="B3" t="inlineStr">
         <is>
           <t>搜索 界面 包含 多个 群组 名称 对应 人数 搜索 无法 正确 展示 ceshi 群组 名称 错误 重复 四次 实际上 两个 相关 群组</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>用户体验</t>
         </is>
       </c>
     </row>
@@ -485,6 +500,11 @@
  定位 分析 软件 运行 产生 大量 缓存数据 造成 手机 内存空间 不足 手机 之前 安装 此款 软件 历史数据 没有 清除 网络 环境 分析 过程 刚刚 网络 延迟 手机 服务器 获取 请求 信息 数据 服务器 响应 信息 发送 手机 端 网络 延迟 出现 响应 数据 不能 正常 接收 闪退</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>不正常退出</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -497,6 +517,11 @@
           <t>群聊 无法 收藏 发送 表情 无法 长 表情 保存 收藏夹 静态 表情 列表 收藏 表情</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>不正常退出</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -509,6 +534,11 @@
           <t>搜索 模糊 匹配 无法 进行 完全 精确 搜索</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -521,6 +551,11 @@
           <t>申请加入 群聊 过程 设置 必须 填写 验证 信息 仍然 填写 申请理由 情况 提交 申请 验证 信息 要求 没有 得到 应有 执行 允许 符合要求 进入 群聊</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -533,6 +568,11 @@
           <t>网络连接 情况 进入 群组 断开 网络 试图 搜索 框中 查找 并未 加入 群组 系统 并未 网络 断开 提示信息 相关</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -545,6 +585,11 @@
           <t>输入 b 查找 群后 查询 页面 下面 没有 提示 完全 部 内容</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -557,6 +602,11 @@
           <t>群组 里 新增 群聊 点击 右上角 加入 群才 第一次 找 不到 入口 右下角 添加 加号 标志 一目了然</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -569,6 +619,11 @@
           <t>软件 重复 加群 请求 群里 情况 系统 仍然 允许 申请加入 同一个 群 困惑 混淆 加群 请求 尚未 处理 新 请求 发送 设计 感到 不便</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -581,6 +636,11 @@
           <t>手机号 注册 新 账号 没有 密码 眼睛 输入 密码 小圆点 无法 查看 输入 具体 密码 容易 用户注册 小心 错 密码 情况 不知情</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -593,6 +653,11 @@
           <t>创建 群聊 修改 昵称 群主 栏 仍然 之前 昵称 表明 群聊 群主 设置 没有 正确 更新 软件 昵称 更改 没有 保存</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -605,6 +670,11 @@
           <t>群聊 小视频 不能 聊天 窗口 播放 转到 应用软件 播放</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -615,6 +685,11 @@
       <c r="B15" t="inlineStr">
         <is>
           <t>群聊 里面 聊天记录 保存 比较 少 页面 太 布局 不好</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
         </is>
       </c>
     </row>
@@ -641,6 +716,11 @@
  -   系统 点击 确定 按钮 没有 反应 反馈 期望 不符</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -653,6 +733,11 @@
           <t>消息 提示 群 里面 发布公告 系统 还会 推送 消息 说 公告 产生 应该 发布公告 知道 系统 推送 消息</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -665,6 +750,11 @@
           <t>群聊 过程 拍照 发送 图片 只能 选择 完整 长宽 图片 进行 发送 不能 图片 进行 裁剪 算是 完整 产生 一定</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -677,6 +767,11 @@
           <t>界面 个人 昵称 进入 好友 主页 发生 一致 变化 第一次 更改 昵称 之后 昵称 明显 错误 表明 系统 处理 昵称 更新 出现 混乱 不一致性 无法 准确 识别 个人信息</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -689,6 +784,11 @@
           <t>群组 创建 图片 试图 创建 新 群组 系统 要求 添加 至少 好友 完成 没有 添加 好友 无法 完成 群组 创建 显然 阻止 这一 软件设计 逻辑 错误 配置</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -701,6 +801,11 @@
           <t>表现 搜索 群组 系统 无法 准确 区分 出 昵称 头像 相同 群组 特别 模糊 匹配 搜索 群号 明确 难以确定 具体 加入 群组</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -713,6 +818,11 @@
           <t>搜索 出现 明显 错误 查找 搜索 匹配 群组 返回 相关 某种 算法 数据源 生成 显然 没有 正确 过滤 出 寻求 信息 意味着 系统 内部 逻辑 数据处理 过程 出现 偏差 进一步 分析 调整 确保 搜索 准确性 相关性</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -725,6 +835,11 @@
           <t>手机 聊天 应用 缺失 具体来说 无法 设置 调整 接收 消息 提示音 振动模式 只能 依赖 手机 媒体 音量控制 实现 一点 集中 注意力 处于 安静 环境 下时 无法 有效 管理 聊天 应用 通知</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -737,6 +852,11 @@
           <t>聊天 消息 进入 界面 历史 消息 消息 没有 发 人员 区分 不利于 辨别 成员 发送 消息</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -749,6 +869,11 @@
           <t>用户界面 设计 明显 编辑 群 名称 删除 部分 文字 系统 没有 单个 字符 进行 删除 成行 删除 文本 意味着 无法 精确 删除 不想 字符 只能 删除 整行 文本 设计 缺陷 修改 输入 群组 名称 遇到困难</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -761,6 +886,11 @@
           <t>点击 群组 查找 群 输入 阿拉伯数字 22 出现 搜索 无关 群组</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -773,6 +903,11 @@
           <t>更换 头像 头像 更改 成功 搜索 头像 没有 改变 手机 查看</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>其他</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -785,6 +920,11 @@
           <t>添加 成员 界面 搜索 框中 输入 关键词 输入 关键词 匹配 无法 正确 展示 输入 相关 信息</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>性能</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -797,6 +937,11 @@
           <t>群聊 界面 进行 手写输入 添加 图片 图片 自动 设置 背景 文字 覆盖 无法 看清 图片 无法 看清 文字</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>页面布局缺陷</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -809,6 +954,11 @@
           <t>创建 群 界面 换行符 群 名称 一部分 系统 换行符 自动 替换 空格 保存 群 信息 原始 输入 布局 一致 具体来说 群 名称 换行 保存 后该 部分 内容 变为 一行 多行 带来 困扰 预期 多行 布局 效果 建议 对此 进行 优化 禁止 创建 群时 换行符 确保 输出 内容 一致性</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>页面布局缺陷</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -821,6 +971,11 @@
           <t>创建 群组 邀请 好友 加入 群组 过程 受 邀请 方 同意 莫名 地拉 入 群组 正常 活动 造成 干扰</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>用户体验</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -833,6 +988,11 @@
           <t>软件测试 过程 发现 发送 手写 内容 相关 点击 发送 手写 内容 系统 发送 内容 提示 再次 点击 发送 按钮 内容 成功 发送 好友 聊天 页面 现象 符合 预期 通常 应该 看到 正在 发送 内容 感到 困惑 无法 预览 发送 内容</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>用户体验</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -845,6 +1005,11 @@
           <t>群组 名称 个人主页 名称 一致 具体表现 群组 默认 昵称 点击 头像 进入 个人主页 名字 更新 修改 名称</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>用户体验</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -857,6 +1022,11 @@
           <t>查找 群 界面 输入 字 段 允许 无限 字符 输入 无法 正确 加载 与此相反 创建 新 群时 系统 限制 字符 数 只能 输入 64 个字符 创建 新群 受限 两个 输入 输出 限制 查找 群 创建 群 表现 出 不同 错误行为</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>用户体验</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -869,6 +1039,11 @@
           <t>群里 聊天 成员 发 语音 无法 听到</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>用户体验</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -881,6 +1056,11 @@
           <t>登录 界面 错误 展示 注册 框而非 登录 框 直觉 期望 不符 切换 账号 找 不到 相应 页面 选项</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>用户体验</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -893,6 +1073,11 @@
           <t>界面设计 过于 简单 过程 感到 压抑</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>用户体验</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -905,6 +1090,11 @@
           <t>注册 界面 输入 限制 过于 严格 仅 允许 11 位 数字 输入 允许 包含 @ 符号 额外 数字 设计 常见 字符 更长 数字 组合 无法 进行 注册 极大</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>用户体验</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -915,6 +1105,11 @@
       <c r="B39" t="inlineStr">
         <is>
           <t>处理 表情 输入 缺陷 发送 一组 表情 表情 完全 输入 准备 发送 之前 出现 历史 表情 记录 感觉 不佳 必现 严重 程度 轻 仍然 造成 负面影响</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>用户体验</t>
         </is>
       </c>
     </row>

</xml_diff>